<commit_message>
Updated p-values to reflect current processed data
</commit_message>
<xml_diff>
--- a/resources/Data/p_value_tables.xlsx
+++ b/resources/Data/p_value_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aashaypatel/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/My_Passport/serotonin_project/to_github/resources/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EC2A13-F9AC-894A-82D0-87C1B95DDCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD99ACD1-B124-B04D-9A5F-AEC288EEA1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18980" xr2:uid="{DF467324-0866-2946-B23A-F3365C304FA2}"/>
+    <workbookView xWindow="4780" yWindow="500" windowWidth="27320" windowHeight="12180" xr2:uid="{DF467324-0866-2946-B23A-F3365C304FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="152">
   <si>
     <t>NaCl (signed rank)</t>
   </si>
@@ -87,55 +85,16 @@
     <t>Normalized Additive Change (NaCl vs 5HT)</t>
   </si>
   <si>
-    <t>0.00407, 13, 16</t>
-  </si>
-  <si>
-    <t>0.24519, 13, 16</t>
-  </si>
-  <si>
-    <t>0.02194, 4, 35</t>
-  </si>
-  <si>
-    <t>0.69397, 4, 35</t>
-  </si>
-  <si>
-    <t>0.00011, 17, 51</t>
-  </si>
-  <si>
-    <t>0.32845, 17, 51</t>
-  </si>
-  <si>
     <t>Figure 1B</t>
   </si>
   <si>
     <t>Figure 1C</t>
   </si>
   <si>
-    <t>Figure 2 (C &amp; G)</t>
-  </si>
-  <si>
-    <t>0.54175, 13</t>
-  </si>
-  <si>
-    <t>7.227e-05, 29</t>
-  </si>
-  <si>
     <t>0.875, 4</t>
   </si>
   <si>
-    <t>2.957e-05, 35</t>
-  </si>
-  <si>
-    <t>0.049129, 39</t>
-  </si>
-  <si>
     <t>0.43476, 17</t>
-  </si>
-  <si>
-    <t>3.1955e-08, 51</t>
-  </si>
-  <si>
-    <t>6.4964e-05, 68</t>
   </si>
   <si>
     <r>
@@ -183,63 +142,15 @@
     </r>
   </si>
   <si>
-    <t>0.16772, 13</t>
-  </si>
-  <si>
     <t>0.00053124, 16</t>
   </si>
   <si>
-    <t>0.0014761, 29</t>
-  </si>
-  <si>
-    <t>0.00029477, 35</t>
-  </si>
-  <si>
-    <t>0.082564, 39</t>
-  </si>
-  <si>
-    <t>0.17729, 17</t>
-  </si>
-  <si>
-    <t>3.2461e-07, 51</t>
-  </si>
-  <si>
-    <t>0.0024381, 68</t>
-  </si>
-  <si>
-    <t>Figure 2 (D &amp; H)</t>
-  </si>
-  <si>
-    <t>Figure 2K</t>
-  </si>
-  <si>
     <t>High vs Low FR (ranksum)</t>
   </si>
   <si>
-    <t>0.038922, 29</t>
-  </si>
-  <si>
-    <t>0.29527, 39</t>
-  </si>
-  <si>
-    <t>0.42345, 68</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Figure 2L</t>
-  </si>
-  <si>
-    <t>0.0033902, 29</t>
-  </si>
-  <si>
-    <t>0.0030918, 39</t>
-  </si>
-  <si>
-    <t>4.023e-05, 68</t>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
@@ -249,19 +160,7 @@
     <t>Figure 3B (E, F, G, H)</t>
   </si>
   <si>
-    <t>0.041434, 29</t>
-  </si>
-  <si>
-    <t>0.18707, 39</t>
-  </si>
-  <si>
     <t>0.98112, 17</t>
-  </si>
-  <si>
-    <t>0.00020572, 51</t>
-  </si>
-  <si>
-    <t>0.021767, 68</t>
   </si>
   <si>
     <r>
@@ -280,17 +179,16 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">0.83936, 13 </t>
+      <t xml:space="preserve">NaCl (signed rank) </t>
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>[E]</t>
+      <t>[D]</t>
     </r>
   </si>
   <si>
@@ -304,20 +202,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>[D]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">NaCl (signed rank) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>[C]</t>
     </r>
   </si>
@@ -350,61 +234,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">0.0052339, 16 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[G]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">0.0083632, 35, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[H]</t>
-    </r>
-  </si>
-  <si>
     <t>Figure 3C</t>
   </si>
   <si>
-    <t>0.78687, 13</t>
-  </si>
-  <si>
-    <t>0.10894, 16</t>
-  </si>
-  <si>
-    <t>0.16717, 29</t>
-  </si>
-  <si>
-    <t>0.011656, 35</t>
-  </si>
-  <si>
-    <t>0.7635, 39</t>
-  </si>
-  <si>
     <t>0.90579, 17</t>
-  </si>
-  <si>
-    <t>0.0028753, 51</t>
-  </si>
-  <si>
-    <t>0.081499, 68</t>
   </si>
   <si>
     <r>
@@ -437,21 +270,9 @@
     <t>0.625, 4</t>
   </si>
   <si>
-    <t>2.0573e-05, 35</t>
-  </si>
-  <si>
     <t>0.049141, 39</t>
   </si>
   <si>
-    <t>0.40743, 17</t>
-  </si>
-  <si>
-    <t>2.194e-08, 51</t>
-  </si>
-  <si>
-    <t>0.00010417, 68</t>
-  </si>
-  <si>
     <t>Figure 3D</t>
   </si>
   <si>
@@ -459,15 +280,6 @@
   </si>
   <si>
     <t>Figure 3 (I &amp; J)</t>
-  </si>
-  <si>
-    <t>0.0027461, 29</t>
-  </si>
-  <si>
-    <t>0.0014639, 39</t>
-  </si>
-  <si>
-    <t>1.1807e-05, 68</t>
   </si>
   <si>
     <r>
@@ -500,60 +312,6 @@
     </r>
   </si>
   <si>
-    <t>0.94604, 13</t>
-  </si>
-  <si>
-    <t>0.00048974, 29</t>
-  </si>
-  <si>
-    <t>5.2785e-06, 35</t>
-  </si>
-  <si>
-    <t>0.044045, 39</t>
-  </si>
-  <si>
-    <t>0.94339, 17</t>
-  </si>
-  <si>
-    <t>6.9221e-09, 51</t>
-  </si>
-  <si>
-    <t>6.1199e-05, 68</t>
-  </si>
-  <si>
-    <t>0.00034539, 29</t>
-  </si>
-  <si>
-    <t>2.7471e-06, 39</t>
-  </si>
-  <si>
-    <t>4.6334e-09, 68</t>
-  </si>
-  <si>
-    <t>1, 13</t>
-  </si>
-  <si>
-    <t>0.0061334, 16</t>
-  </si>
-  <si>
-    <t>0.013224, 29</t>
-  </si>
-  <si>
-    <t>7.9013e-05, 35</t>
-  </si>
-  <si>
-    <t>0.060822, 39</t>
-  </si>
-  <si>
-    <t>0.72256, 17</t>
-  </si>
-  <si>
-    <t>1.5929e-06, 51</t>
-  </si>
-  <si>
-    <t>0.00071187, 68</t>
-  </si>
-  <si>
     <t>Figure 4 [MI Value: Drug Condition]</t>
   </si>
   <si>
@@ -563,49 +321,10 @@
     <t>Figure 4 [Correlation: Drug Condition]</t>
   </si>
   <si>
-    <t>0.23011, 29</t>
-  </si>
-  <si>
-    <t>0.012492, 39</t>
-  </si>
-  <si>
-    <t>0.0070459, 68</t>
-  </si>
-  <si>
     <t>Figure 4 [MI Value: FR Control]</t>
   </si>
   <si>
     <t>Figure S1B (E, F, G, H)</t>
-  </si>
-  <si>
-    <t>0.03725, 29</t>
-  </si>
-  <si>
-    <t>0.27667, 39</t>
-  </si>
-  <si>
-    <t>0.83131, 17</t>
-  </si>
-  <si>
-    <t>0.00021347, 51</t>
-  </si>
-  <si>
-    <t>0.017341, 68</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">0.78687, 13 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[E]</t>
-    </r>
   </si>
   <si>
     <r>
@@ -623,58 +342,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">0.019971, 16 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[G]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">0.0033693, 35 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[H]</t>
-    </r>
-  </si>
-  <si>
     <t>0.83936, 13</t>
-  </si>
-  <si>
-    <t>0.078731, 16</t>
-  </si>
-  <si>
-    <t>0.1303, 29</t>
-  </si>
-  <si>
-    <t>0.0030305, 35</t>
-  </si>
-  <si>
-    <t>0.83499, 39</t>
-  </si>
-  <si>
-    <t>0.61915, 17</t>
-  </si>
-  <si>
-    <t>0.00079164, 51</t>
-  </si>
-  <si>
-    <t>0.10337, 68</t>
   </si>
   <si>
     <t>Figure S1C</t>
@@ -706,22 +374,346 @@
     <t>0.010195, 39</t>
   </si>
   <si>
-    <t>2.444e-08, 51</t>
-  </si>
-  <si>
-    <t>0.00013129, 68</t>
-  </si>
-  <si>
     <t>Figure S1D</t>
   </si>
   <si>
     <t>Figure S1 (I &amp; J)</t>
   </si>
   <si>
-    <t>0.0016542, 29</t>
-  </si>
-  <si>
-    <t>0.0021399, 39</t>
+    <t>0.00404, 4, 8</t>
+  </si>
+  <si>
+    <t>0.07745, 3, 23</t>
+  </si>
+  <si>
+    <t>0.00120, 7, 31</t>
+  </si>
+  <si>
+    <t>0.40743, 7, 31</t>
+  </si>
+  <si>
+    <t>0.33550, 3, 23</t>
+  </si>
+  <si>
+    <t>0.56970, 4, 8</t>
+  </si>
+  <si>
+    <t>Figure 2 (D &amp; H) (Gamma)</t>
+  </si>
+  <si>
+    <t>0.45483, 13</t>
+  </si>
+  <si>
+    <t>0.0010868, 29</t>
+  </si>
+  <si>
+    <t>0.125, 4</t>
+  </si>
+  <si>
+    <t>4.2243e-05, 35</t>
+  </si>
+  <si>
+    <t>0.035174, 39</t>
+  </si>
+  <si>
+    <t>0.79459, 17</t>
+  </si>
+  <si>
+    <t>4.8866e-08, 51</t>
+  </si>
+  <si>
+    <t>0.00060919, 68</t>
+  </si>
+  <si>
+    <t>Figure 2 (C &amp; G) (Low-Freq)</t>
+  </si>
+  <si>
+    <t>Figure 2L (Gamma)</t>
+  </si>
+  <si>
+    <t>0.011062, 29</t>
+  </si>
+  <si>
+    <t>0.012992, 39</t>
+  </si>
+  <si>
+    <t>0.00051914, 68</t>
+  </si>
+  <si>
+    <t>0.6355, 13</t>
+  </si>
+  <si>
+    <t>0.00014867, 29</t>
+  </si>
+  <si>
+    <t>3.1773e-05, 35</t>
+  </si>
+  <si>
+    <t>0.05471, 39</t>
+  </si>
+  <si>
+    <t>0.55403, 17</t>
+  </si>
+  <si>
+    <t>3.029e-08, 51</t>
+  </si>
+  <si>
+    <t>0.00013127, 68</t>
+  </si>
+  <si>
+    <t>Figure 2K (Low-Freq)</t>
+  </si>
+  <si>
+    <t>0.020099, 29</t>
+  </si>
+  <si>
+    <t>0.19435, 39</t>
+  </si>
+  <si>
+    <t>0.41291, 68</t>
+  </si>
+  <si>
+    <t>0.00092998, 29</t>
+  </si>
+  <si>
+    <t>3.8575e-06, 35</t>
+  </si>
+  <si>
+    <t>0.68741, 17</t>
+  </si>
+  <si>
+    <t>4.9441e-09, 51</t>
+  </si>
+  <si>
+    <t>7.3196e-05, 68</t>
+  </si>
+  <si>
+    <t>0.89258, 13</t>
+  </si>
+  <si>
+    <t>0.0044554, 16</t>
+  </si>
+  <si>
+    <t>0.016849, 29</t>
+  </si>
+  <si>
+    <t>1, 4</t>
+  </si>
+  <si>
+    <t>3.9367e-05, 35</t>
+  </si>
+  <si>
+    <t>0.75831, 17</t>
+  </si>
+  <si>
+    <t>7.4523e-07, 51</t>
+  </si>
+  <si>
+    <t>0.00057824, 68</t>
+  </si>
+  <si>
+    <t>0.00044179, 29</t>
+  </si>
+  <si>
+    <t>0.0002056, 39</t>
+  </si>
+  <si>
+    <t>2.5075e-07, 68</t>
+  </si>
+  <si>
+    <t>0.006308, 68</t>
+  </si>
+  <si>
+    <t>0.020529, 39</t>
+  </si>
+  <si>
+    <t>0.1274, 29</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1, 13 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[E]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0.043733, 16 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[G]</t>
+    </r>
+  </si>
+  <si>
+    <t>0.051003, 29</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0.0041523, 35 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[H]</t>
+    </r>
+  </si>
+  <si>
+    <t>0.31961, 39</t>
+  </si>
+  <si>
+    <t>0.00040964, 51</t>
+  </si>
+  <si>
+    <t>0.020193, 68</t>
+  </si>
+  <si>
+    <t>0.58789, 13</t>
+  </si>
+  <si>
+    <t>0.062671, 16</t>
+  </si>
+  <si>
+    <t>0.18106, 29</t>
+  </si>
+  <si>
+    <t>0.0011163, 35</t>
+  </si>
+  <si>
+    <t>0.69397, 39</t>
+  </si>
+  <si>
+    <t>0.46311, 17</t>
+  </si>
+  <si>
+    <t>0.00034272, 51</t>
+  </si>
+  <si>
+    <t>0.086579, 68</t>
+  </si>
+  <si>
+    <t>2.7216e-08, 51</t>
+  </si>
+  <si>
+    <t>0.00012395, 68</t>
+  </si>
+  <si>
+    <t>0.001536, 29</t>
+  </si>
+  <si>
+    <t>0.0016902, 39</t>
+  </si>
+  <si>
+    <t>7.2914e-06, 68</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0.89258, 13 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[E]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0.0097255, 16 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[G]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0.006232, 35 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[H]</t>
+    </r>
+  </si>
+  <si>
+    <t>0.15799, 39</t>
+  </si>
+  <si>
+    <t>0.00025653, 51</t>
+  </si>
+  <si>
+    <t>0.0029472, 29</t>
+  </si>
+  <si>
+    <t>0.0018585, 39</t>
+  </si>
+  <si>
+    <t>1.6489e-05, 68</t>
+  </si>
+  <si>
+    <t>0.038607, 16</t>
+  </si>
+  <si>
+    <t>0.091347, 29</t>
+  </si>
+  <si>
+    <t>0.021843, 35</t>
+  </si>
+  <si>
+    <t>0.62693, 39</t>
+  </si>
+  <si>
+    <t>0.0025423, 51</t>
+  </si>
+  <si>
+    <t>0.06155, 68</t>
+  </si>
+  <si>
+    <t>3.4141e-05, 35</t>
+  </si>
+  <si>
+    <t>0.49246, 17</t>
+  </si>
+  <si>
+    <t>3.196e-08, 51</t>
+  </si>
+  <si>
+    <t>0.00015587, 68</t>
   </si>
 </sst>
 </file>
@@ -1156,36 +1148,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1249,6 +1211,36 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1264,10 +1256,11 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1282,6 +1275,80 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1319,20 +1386,257 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -1343,15 +1647,10 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -1361,6 +1660,81 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1379,16 +1753,10 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -1407,7 +1775,53 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color auto="1"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -1426,98 +1840,82 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
         <color auto="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -1576,67 +1974,34 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color auto="1"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1650,216 +2015,81 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -1878,52 +2108,178 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color auto="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -1952,499 +2308,135 @@
     <dxf>
       <font>
         <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color auto="1"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color auto="1"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2474,13 +2466,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{21C35471-0FB1-2546-99EB-AB7E318F157A}" name="Table1" displayName="Table1" ref="A4:D7" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{21C35471-0FB1-2546-99EB-AB7E318F157A}" name="Table1" displayName="Table1" ref="A4:D7" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
   <autoFilter ref="A4:D7" xr:uid="{21C35471-0FB1-2546-99EB-AB7E318F157A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83721C0E-46A7-3743-A6D2-91CB9DFD484A}" name="p value, ndrug" dataDxfId="97"/>
-    <tableColumn id="2" xr3:uid="{D9483881-C632-F14D-A80E-9DEB12281230}" name="NaCl (signed rank)" dataDxfId="96"/>
-    <tableColumn id="3" xr3:uid="{21546308-968D-D74F-9D07-C5C6766C34C9}" name="5HT (signed rank)" dataDxfId="95"/>
-    <tableColumn id="4" xr3:uid="{BD89FE4B-1908-634E-88BD-F6D4573DAEA8}" name="NaCl vs 5HT (ranksum)" dataDxfId="94"/>
+    <tableColumn id="1" xr3:uid="{83721C0E-46A7-3743-A6D2-91CB9DFD484A}" name="p value, ndrug" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{D9483881-C632-F14D-A80E-9DEB12281230}" name="NaCl (signed rank)" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{21546308-968D-D74F-9D07-C5C6766C34C9}" name="5HT (signed rank)" dataDxfId="93"/>
+    <tableColumn id="4" xr3:uid="{BD89FE4B-1908-634E-88BD-F6D4573DAEA8}" name="NaCl vs 5HT (ranksum)" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2500,7 +2492,7 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{CB6BB37A-DF8A-3F4A-8C7C-7068E706057F}" name="Table12" displayName="Table12" ref="A67:B70" totalsRowShown="0" headerRowDxfId="35" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{CB6BB37A-DF8A-3F4A-8C7C-7068E706057F}" name="Table12" displayName="Table12" ref="A67:B70" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A67:B70" xr:uid="{CB6BB37A-DF8A-3F4A-8C7C-7068E706057F}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C8666905-17ED-E042-AB5B-A635586A0533}" name="  " dataDxfId="34"/>
@@ -2524,24 +2516,24 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E6DD0737-D28F-1F4C-B53C-A4A6EF25F271}" name="Table14" displayName="Table14" ref="A79:B82" totalsRowShown="0" headerRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E6DD0737-D28F-1F4C-B53C-A4A6EF25F271}" name="Table14" displayName="Table14" ref="A79:B82" totalsRowShown="0" headerRowDxfId="27">
   <autoFilter ref="A79:B82" xr:uid="{E6DD0737-D28F-1F4C-B53C-A4A6EF25F271}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0C58147E-AC15-A545-BC38-F2E61BDA7CE8}" name=" " dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{8D6555BD-5093-5E4F-BFFF-C177158E876B}" name="High vs Low FR (ranksum)" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{0C58147E-AC15-A545-BC38-F2E61BDA7CE8}" name=" " dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{8D6555BD-5093-5E4F-BFFF-C177158E876B}" name="High vs Low FR (ranksum)" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{FF92885A-A117-BD46-9632-075EE49B7727}" name="Table15" displayName="Table15" ref="A86:D89" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{FF92885A-A117-BD46-9632-075EE49B7727}" name="Table15" displayName="Table15" ref="A86:D89" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A86:D89" xr:uid="{FF92885A-A117-BD46-9632-075EE49B7727}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{34D4DF3E-AE3E-464E-95DE-24DB9779A9AB}" name="p value, ndrug" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{BC707775-30D0-9342-B7C6-5C185C8EEE6E}" name="NaCl (signed rank)" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{E4EDEEC3-D74B-A049-831E-AE3835B1654C}" name="5HT (signed rank)" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{E84C0DB0-55B0-FE42-ABCC-3D367094A1CB}" name="NaCl vs 5HT (ranksum)" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{34D4DF3E-AE3E-464E-95DE-24DB9779A9AB}" name="p value, ndrug" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{BC707775-30D0-9342-B7C6-5C185C8EEE6E}" name="NaCl (signed rank)" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{E4EDEEC3-D74B-A049-831E-AE3835B1654C}" name="5HT (signed rank)" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{E84C0DB0-55B0-FE42-ABCC-3D367094A1CB}" name="NaCl vs 5HT (ranksum)" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2589,38 +2581,38 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4403CAAD-D4E2-FE4F-A9F8-F40989562CE3}" name="Table2" displayName="Table2" ref="A10:C13" totalsRowShown="0" headerRowDxfId="88" dataDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4403CAAD-D4E2-FE4F-A9F8-F40989562CE3}" name="Table2" displayName="Table2" ref="A10:C13" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90">
   <autoFilter ref="A10:C13" xr:uid="{4403CAAD-D4E2-FE4F-A9F8-F40989562CE3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6F6323EB-F59E-A840-B360-53A0BFC0B09F}" name="p value, nNaCl, n5HT" dataDxfId="91"/>
-    <tableColumn id="2" xr3:uid="{9886D83A-34F3-C049-A463-BE2499DBB188}" name="Relative Gain Change (NaCl vs 5HT)" dataDxfId="90"/>
-    <tableColumn id="3" xr3:uid="{9457F94D-8C5D-4943-A6A6-79262CF1E388}" name="Normalized Additive Change (NaCl vs 5HT)" dataDxfId="89"/>
+    <tableColumn id="1" xr3:uid="{6F6323EB-F59E-A840-B360-53A0BFC0B09F}" name="p value, nNaCl, n5HT" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{9886D83A-34F3-C049-A463-BE2499DBB188}" name="Relative Gain Change (NaCl vs 5HT)" dataDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{9457F94D-8C5D-4943-A6A6-79262CF1E388}" name="Normalized Additive Change (NaCl vs 5HT)" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2A9F3E2A-8A2A-B44B-B5F7-D7C12ABB647C}" name="Table3" displayName="Table3" ref="A17:D20" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2A9F3E2A-8A2A-B44B-B5F7-D7C12ABB647C}" name="Table3" displayName="Table3" ref="A17:D20" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
   <autoFilter ref="A17:D20" xr:uid="{2A9F3E2A-8A2A-B44B-B5F7-D7C12ABB647C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{14955E8D-710A-BB4F-BC6D-9BDAFECDBCFD}" name="p value, ndrug" dataDxfId="86"/>
-    <tableColumn id="2" xr3:uid="{7D4CC906-FBF8-B044-A55D-2C67202F20EF}" name="NaCl (signed rank) [C]" dataDxfId="85"/>
-    <tableColumn id="3" xr3:uid="{61FD05FB-45C3-FE4F-BCDD-1E231027F3D0}" name="5HT (signed rank) [G]" dataDxfId="84"/>
-    <tableColumn id="4" xr3:uid="{976FCC62-D07D-424F-8724-8802CBCBF352}" name="NaCl vs 5HT (ranksum)" dataDxfId="83"/>
+    <tableColumn id="1" xr3:uid="{14955E8D-710A-BB4F-BC6D-9BDAFECDBCFD}" name="p value, ndrug" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{7D4CC906-FBF8-B044-A55D-2C67202F20EF}" name="NaCl (signed rank) [C]" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{61FD05FB-45C3-FE4F-BCDD-1E231027F3D0}" name="5HT (signed rank) [G]" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{976FCC62-D07D-424F-8724-8802CBCBF352}" name="NaCl vs 5HT (ranksum)" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9DF7E1A3-41E0-8848-93AC-CCAB4A8782EA}" name="Table4" displayName="Table4" ref="A23:D26" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9DF7E1A3-41E0-8848-93AC-CCAB4A8782EA}" name="Table4" displayName="Table4" ref="A23:D26" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
   <autoFilter ref="A23:D26" xr:uid="{9DF7E1A3-41E0-8848-93AC-CCAB4A8782EA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{43B21679-5A01-4140-B08C-59ADA589D709}" name="p value, ndrug" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{083002A5-A730-1043-916E-250C61D63CD4}" name="NaCl (signed rank) [D]" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{E8E45B1A-B074-9247-B32D-BCAB5F9EBBDC}" name="5HT (signed rank) [H]" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{1A7477FA-876E-EC4C-8FC6-9F01492F92CC}" name="NaCl vs 5HT (ranksum)" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{43B21679-5A01-4140-B08C-59ADA589D709}" name="p value, ndrug" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{083002A5-A730-1043-916E-250C61D63CD4}" name="NaCl (signed rank) [D]" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{E8E45B1A-B074-9247-B32D-BCAB5F9EBBDC}" name="5HT (signed rank) [H]" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{1A7477FA-876E-EC4C-8FC6-9F01492F92CC}" name="NaCl vs 5HT (ranksum)" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2630,17 +2622,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5CEDF8AB-FD4B-6F4B-8A4F-377FE7A1E82B}" name="Table5" displayName="Table5" ref="A29:D32" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
   <autoFilter ref="A29:D32" xr:uid="{5CEDF8AB-FD4B-6F4B-8A4F-377FE7A1E82B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A0FECC8F-57C8-D045-BFA1-E74DC60CA8A6}" name=" " dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{83C2F8D3-2A0F-5E40-944E-FC16513E7441}" name="High vs Low FR (ranksum)" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{B06939D4-4FB3-7946-8C18-9C81581FF0F0}" name="  " dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{CB152F73-523C-EC48-BCDE-3DBA535AF776}" name="High vs Low FR (ranksum) " dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{A0FECC8F-57C8-D045-BFA1-E74DC60CA8A6}" name=" " dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{83C2F8D3-2A0F-5E40-944E-FC16513E7441}" name="High vs Low FR (ranksum)" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{B06939D4-4FB3-7946-8C18-9C81581FF0F0}" name="  " dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{CB152F73-523C-EC48-BCDE-3DBA535AF776}" name="High vs Low FR (ranksum) " dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C5321602-2C62-6441-BD49-34843DC5EC9E}" name="Table6" displayName="Table6" ref="A36:D39" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C5321602-2C62-6441-BD49-34843DC5EC9E}" name="Table6" displayName="Table6" ref="A36:D39" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <autoFilter ref="A36:D39" xr:uid="{C5321602-2C62-6441-BD49-34843DC5EC9E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{1F814F2A-B411-9143-91B9-4B3599DB13CF}" name="p value, ndrug" dataDxfId="66"/>
@@ -2653,13 +2645,13 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AF7CAE5F-4050-494B-8444-4010FD9A9503}" name="Table7" displayName="Table7" ref="A42:D45" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AF7CAE5F-4050-494B-8444-4010FD9A9503}" name="Table7" displayName="Table7" ref="A42:D45" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="A42:D45" xr:uid="{AF7CAE5F-4050-494B-8444-4010FD9A9503}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8B916019-25D3-3D45-9925-267A0402C4F8}" name="p value, ndrug" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{61736AC6-9797-5B48-B183-3B6215218DF8}" name="NaCl (signed rank)" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{DAC507F1-97A1-DA42-A2DF-32A43755F789}" name="5HT (signed rank)" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{A3523461-2D77-EE4C-B139-F74D1601F9DA}" name="NaCl vs 5HT (ranksum)" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{8B916019-25D3-3D45-9925-267A0402C4F8}" name="p value, ndrug" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{61736AC6-9797-5B48-B183-3B6215218DF8}" name="NaCl (signed rank)" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{DAC507F1-97A1-DA42-A2DF-32A43755F789}" name="5HT (signed rank)" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{A3523461-2D77-EE4C-B139-F74D1601F9DA}" name="NaCl vs 5HT (ranksum)" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2669,25 +2661,25 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0C5BDE58-1E6E-384C-A301-88BC3A7CF412}" name="Table8" displayName="Table8" ref="A48:H51" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
   <autoFilter ref="A48:H51" xr:uid="{0C5BDE58-1E6E-384C-A301-88BC3A7CF412}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5EA9C801-7A12-FA47-9993-79019D358F40}" name="p value, ndrug" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{B0AC27D2-E46F-DD43-A6E6-70FCFEC67CCF}" name="NaCl (signed rank)" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{3405FAE7-1917-E54E-AFF6-4688DF55E888}" name="5HT (signed rank)" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{C4701D78-F5C1-8F44-B509-9C65927C23EA}" name="NaCl vs 5HT (ranksum)" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{2F13EFC0-F883-C94A-8B8D-AE9876F7A632}" name="Pearson Coefficient (NaCl)" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{FE0F23F0-7EFF-0F42-BEB6-61A6C30BEECE}" name="P-val (Pearson NaCl)" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{3409405C-6EC3-FA4F-82E9-0BF2E7CF2C8C}" name="Pearson Coefficient (5HT)" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{62A00288-B558-734C-AA35-F093E3D1CBB7}" name="P-val (Pearson 5HT)" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{5EA9C801-7A12-FA47-9993-79019D358F40}" name="p value, ndrug" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{B0AC27D2-E46F-DD43-A6E6-70FCFEC67CCF}" name="NaCl (signed rank)" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{3405FAE7-1917-E54E-AFF6-4688DF55E888}" name="5HT (signed rank)" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{C4701D78-F5C1-8F44-B509-9C65927C23EA}" name="NaCl vs 5HT (ranksum)" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{2F13EFC0-F883-C94A-8B8D-AE9876F7A632}" name="Pearson Coefficient (NaCl)" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{FE0F23F0-7EFF-0F42-BEB6-61A6C30BEECE}" name="P-val (Pearson NaCl)" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{3409405C-6EC3-FA4F-82E9-0BF2E7CF2C8C}" name="Pearson Coefficient (5HT)" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{62A00288-B558-734C-AA35-F093E3D1CBB7}" name="P-val (Pearson 5HT)" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{48CAD425-0C99-8048-AF71-3B8C84DE14B0}" name="Table9" displayName="Table9" ref="A54:B57" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{48CAD425-0C99-8048-AF71-3B8C84DE14B0}" name="Table9" displayName="Table9" ref="A54:B57" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A54:B57" xr:uid="{48CAD425-0C99-8048-AF71-3B8C84DE14B0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{ABF2BE29-2111-6C46-AB1E-A3D7A182CFB9}" name="  " dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{C2EDD93A-A485-674E-B1D4-92AF4ADACF33}" name="High vs Low FR (ranksum)" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{ABF2BE29-2111-6C46-AB1E-A3D7A182CFB9}" name="  " dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{C2EDD93A-A485-674E-B1D4-92AF4ADACF33}" name="High vs Low FR (ranksum)" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2992,11 +2984,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7AD4EF-B60C-B945-BD48-3B2B2FC6C51E}">
   <dimension ref="A3:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="101" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.83203125" style="4" bestFit="1" customWidth="1"/>
@@ -3011,12 +3003,12 @@
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -3072,12 +3064,12 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
@@ -3091,10 +3083,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3102,10 +3094,10 @@
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3113,26 +3105,26 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>2</v>
@@ -3143,13 +3135,13 @@
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -3157,13 +3149,13 @@
         <v>7</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3171,29 +3163,29 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>2</v>
@@ -3204,13 +3196,13 @@
         <v>3</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -3218,13 +3210,13 @@
         <v>7</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -3232,35 +3224,35 @@
         <v>11</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -3268,13 +3260,13 @@
         <v>3</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -3282,13 +3274,13 @@
         <v>7</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -3296,23 +3288,23 @@
         <v>11</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>0</v>
@@ -3329,13 +3321,13 @@
         <v>3</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>69</v>
+        <v>135</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -3343,13 +3335,13 @@
         <v>7</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>59</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -3357,23 +3349,23 @@
         <v>11</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>61</v>
+        <v>138</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>0</v>
@@ -3390,13 +3382,13 @@
         <v>3</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>74</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -3404,13 +3396,13 @@
         <v>7</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>76</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -3418,23 +3410,23 @@
         <v>11</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>79</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>0</v>
@@ -3446,16 +3438,16 @@
         <v>2</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -3463,25 +3455,25 @@
         <v>3</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="E49" s="9">
-        <v>0.10183</v>
+        <v>0.16904</v>
       </c>
       <c r="F49" s="9">
-        <v>0.74061999999999995</v>
+        <v>0.58089999999999997</v>
       </c>
       <c r="G49" s="9">
-        <v>0.24557000000000001</v>
+        <v>0.20805999999999999</v>
       </c>
       <c r="H49" s="9">
-        <v>0.35926999999999998</v>
+        <v>0.43936999999999998</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -3489,25 +3481,25 @@
         <v>7</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
       <c r="E50" s="9">
-        <v>0.90607000000000004</v>
+        <v>0.87673999999999996</v>
       </c>
       <c r="F50" s="9">
-        <v>9.3932000000000002E-2</v>
+        <v>0.12325999999999999</v>
       </c>
       <c r="G50" s="9">
-        <v>0.70743999999999996</v>
+        <v>0.71475999999999995</v>
       </c>
       <c r="H50" s="10">
-        <v>2.0153999999999998E-6</v>
+        <v>1.4107999999999999E-6</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -3515,54 +3507,54 @@
         <v>11</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>89</v>
+        <v>150</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>90</v>
+        <v>151</v>
       </c>
       <c r="E51" s="9">
-        <v>0.22453999999999999</v>
+        <v>0.25755</v>
       </c>
       <c r="F51" s="9">
-        <v>0.38624999999999998</v>
+        <v>0.31829000000000002</v>
       </c>
       <c r="G51" s="9">
-        <v>0.55369999999999997</v>
+        <v>0.53483999999999998</v>
       </c>
       <c r="H51" s="10">
-        <v>2.5015999999999999E-5</v>
+        <v>5.2726999999999998E-5</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -3570,17 +3562,17 @@
         <v>11</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>119</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>0</v>
@@ -3597,13 +3589,13 @@
         <v>3</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -3611,13 +3603,13 @@
         <v>7</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>102</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -3625,26 +3617,26 @@
         <v>11</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>118</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -3652,7 +3644,7 @@
         <v>3</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -3660,7 +3652,7 @@
         <v>7</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -3668,17 +3660,17 @@
         <v>11</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>117</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>0</v>
@@ -3695,13 +3687,13 @@
         <v>3</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -3709,13 +3701,13 @@
         <v>7</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>113</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -3723,26 +3715,26 @@
         <v>11</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
-        <v>123</v>
+        <v>52</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -3750,7 +3742,7 @@
         <v>3</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -3758,7 +3750,7 @@
         <v>7</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -3766,17 +3758,17 @@
         <v>11</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
-        <v>124</v>
+        <v>53</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>0</v>
@@ -3793,13 +3785,13 @@
         <v>3</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -3807,13 +3799,13 @@
         <v>7</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>131</v>
+        <v>54</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -3821,23 +3813,23 @@
         <v>11</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
-        <v>142</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>0</v>
@@ -3854,13 +3846,13 @@
         <v>3</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -3868,13 +3860,13 @@
         <v>7</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -3882,23 +3874,23 @@
         <v>11</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
-        <v>150</v>
+        <v>62</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>0</v>
@@ -3910,16 +3902,16 @@
         <v>2</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -3927,25 +3919,25 @@
         <v>3</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>144</v>
+        <v>58</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>145</v>
+        <v>59</v>
       </c>
       <c r="E99" s="3">
-        <v>0.29854000000000003</v>
+        <v>0.28042</v>
       </c>
       <c r="F99" s="3">
-        <v>0.32179999999999997</v>
+        <v>0.35341</v>
       </c>
       <c r="G99" s="3">
-        <v>0.21468000000000001</v>
+        <v>3.5858999999999999E-3</v>
       </c>
       <c r="H99" s="3">
-        <v>0.42460999999999999</v>
+        <v>0.98948000000000003</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -3953,25 +3945,25 @@
         <v>7</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>146</v>
+        <v>60</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>147</v>
+        <v>61</v>
       </c>
       <c r="E100" s="3">
-        <v>0.59414</v>
+        <v>0.60348000000000002</v>
       </c>
       <c r="F100" s="3">
-        <v>0.40586</v>
+        <v>0.39651999999999998</v>
       </c>
       <c r="G100" s="3">
-        <v>0.71228999999999998</v>
+        <v>0.72062000000000004</v>
       </c>
       <c r="H100" s="11">
-        <v>1.5929E-6</v>
+        <v>1.0519E-6</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -3979,54 +3971,54 @@
         <v>11</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="E101" s="3">
-        <v>0.31519999999999998</v>
+        <v>0.30176999999999998</v>
       </c>
       <c r="F101" s="3">
-        <v>0.21783</v>
+        <v>0.23913999999999999</v>
       </c>
       <c r="G101" s="3">
-        <v>0.54752999999999996</v>
+        <v>0.46639999999999998</v>
       </c>
       <c r="H101" s="11">
-        <v>3.2076000000000003E-5</v>
+        <v>5.6138E-4</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
-        <v>151</v>
+        <v>63</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -4034,7 +4026,7 @@
         <v>11</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated p-values for figures using data sets with additional fields
</commit_message>
<xml_diff>
--- a/resources/Data/p_value_tables.xlsx
+++ b/resources/Data/p_value_tables.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/My_Passport/serotonin_project/to_github/resources/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\serotonin_project\to_github\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD99ACD1-B124-B04D-9A5F-AEC288EEA1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D77B7EB-DA9B-4EA5-A458-0719738B82AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="500" windowWidth="27320" windowHeight="12180" xr2:uid="{DF467324-0866-2946-B23A-F3365C304FA2}"/>
+    <workbookView xWindow="-111" yWindow="746" windowWidth="19748" windowHeight="13114" xr2:uid="{DF467324-0866-2946-B23A-F3365C304FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="158">
   <si>
     <t>NaCl (signed rank)</t>
   </si>
@@ -235,9 +236,6 @@
   </si>
   <si>
     <t>Figure 3C</t>
-  </si>
-  <si>
-    <t>0.90579, 17</t>
   </si>
   <si>
     <r>
@@ -264,9 +262,6 @@
     <t>P-val (Pearson 5HT)</t>
   </si>
   <si>
-    <t>0.00021092, 29</t>
-  </si>
-  <si>
     <t>0.625, 4</t>
   </si>
   <si>
@@ -380,24 +375,6 @@
     <t>Figure S1 (I &amp; J)</t>
   </si>
   <si>
-    <t>0.00404, 4, 8</t>
-  </si>
-  <si>
-    <t>0.07745, 3, 23</t>
-  </si>
-  <si>
-    <t>0.00120, 7, 31</t>
-  </si>
-  <si>
-    <t>0.40743, 7, 31</t>
-  </si>
-  <si>
-    <t>0.33550, 3, 23</t>
-  </si>
-  <si>
-    <t>0.56970, 4, 8</t>
-  </si>
-  <si>
     <t>Figure 2 (D &amp; H) (Gamma)</t>
   </si>
   <si>
@@ -410,21 +387,9 @@
     <t>0.125, 4</t>
   </si>
   <si>
-    <t>4.2243e-05, 35</t>
-  </si>
-  <si>
-    <t>0.035174, 39</t>
-  </si>
-  <si>
     <t>0.79459, 17</t>
   </si>
   <si>
-    <t>4.8866e-08, 51</t>
-  </si>
-  <si>
-    <t>0.00060919, 68</t>
-  </si>
-  <si>
     <t>Figure 2 (C &amp; G) (Low-Freq)</t>
   </si>
   <si>
@@ -438,27 +403,6 @@
   </si>
   <si>
     <t>0.00051914, 68</t>
-  </si>
-  <si>
-    <t>0.6355, 13</t>
-  </si>
-  <si>
-    <t>0.00014867, 29</t>
-  </si>
-  <si>
-    <t>3.1773e-05, 35</t>
-  </si>
-  <si>
-    <t>0.05471, 39</t>
-  </si>
-  <si>
-    <t>0.55403, 17</t>
-  </si>
-  <si>
-    <t>3.029e-08, 51</t>
-  </si>
-  <si>
-    <t>0.00013127, 68</t>
   </si>
   <si>
     <t>Figure 2K (Low-Freq)</t>
@@ -641,8 +585,80 @@
     </r>
   </si>
   <si>
+    <t>0.0029472, 29</t>
+  </si>
+  <si>
+    <t>0.0018585, 39</t>
+  </si>
+  <si>
+    <t>1.6489e-05, 68</t>
+  </si>
+  <si>
+    <t>Differences in Low-Freq Effect (Panel 2G vs 2K)</t>
+  </si>
+  <si>
+    <t>Differences in Gamma Effect (Panel 2H vs 2L)</t>
+  </si>
+  <si>
+    <t>0.0016, 16</t>
+  </si>
+  <si>
+    <t>0.0106, 34</t>
+  </si>
+  <si>
+    <t>4.7244e-05, 50</t>
+  </si>
+  <si>
+    <t>6.5508e-05, 34</t>
+  </si>
+  <si>
+    <t>0.038538, 38</t>
+  </si>
+  <si>
+    <t>7.3784e-08, 50</t>
+  </si>
+  <si>
+    <t>0.00069065, 67</t>
+  </si>
+  <si>
+    <t>4.8984e-05, 34</t>
+  </si>
+  <si>
+    <t>0.060269, 38</t>
+  </si>
+  <si>
+    <t>0.02398, 4, 10</t>
+  </si>
+  <si>
+    <t>0.01294, 4, 30</t>
+  </si>
+  <si>
+    <t>0.00034, 8, 40</t>
+  </si>
+  <si>
+    <t>0.18781, 4, 10</t>
+  </si>
+  <si>
+    <t>0.57463, 4, 30</t>
+  </si>
+  <si>
+    <t>0.51562, 8, 40</t>
+  </si>
+  <si>
+    <t>7.227e-05, 29</t>
+  </si>
+  <si>
+    <t>0.40743, 17</t>
+  </si>
+  <si>
+    <t>4.7902e-08, 50</t>
+  </si>
+  <si>
+    <t>8.1211e-05, 67</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">0.0097255, 16 </t>
+      <t xml:space="preserve">0.0044554, 16 </t>
     </r>
     <r>
       <rPr>
@@ -657,7 +673,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">0.006232, 35 </t>
+      <t xml:space="preserve">0.0039425, 35 </t>
     </r>
     <r>
       <rPr>
@@ -671,56 +687,59 @@
     </r>
   </si>
   <si>
-    <t>0.15799, 39</t>
-  </si>
-  <si>
-    <t>0.00025653, 51</t>
-  </si>
-  <si>
-    <t>0.0029472, 29</t>
-  </si>
-  <si>
-    <t>0.0018585, 39</t>
-  </si>
-  <si>
-    <t>1.6489e-05, 68</t>
-  </si>
-  <si>
-    <t>0.038607, 16</t>
-  </si>
-  <si>
-    <t>0.091347, 29</t>
-  </si>
-  <si>
-    <t>0.021843, 35</t>
-  </si>
-  <si>
-    <t>0.62693, 39</t>
-  </si>
-  <si>
-    <t>0.0025423, 51</t>
-  </si>
-  <si>
-    <t>0.06155, 68</t>
-  </si>
-  <si>
-    <t>3.4141e-05, 35</t>
-  </si>
-  <si>
-    <t>0.49246, 17</t>
-  </si>
-  <si>
-    <t>3.196e-08, 51</t>
-  </si>
-  <si>
-    <t>0.00015587, 68</t>
+    <t>0.18707, 39</t>
+  </si>
+  <si>
+    <t>0.00014145, 51</t>
+  </si>
+  <si>
+    <t>0.019444, 68</t>
+  </si>
+  <si>
+    <t>0.41431, 13</t>
+  </si>
+  <si>
+    <t>0.00010404, 29</t>
+  </si>
+  <si>
+    <t>2.3807e-05, 35</t>
+  </si>
+  <si>
+    <t>0.33183, 17</t>
+  </si>
+  <si>
+    <t>2.444e-08, 51</t>
+  </si>
+  <si>
+    <t>9.8265e-05, 68</t>
+  </si>
+  <si>
+    <t>0.14181, 29</t>
+  </si>
+  <si>
+    <t>0.0019182, 51</t>
+  </si>
+  <si>
+    <t>0.055719, 16</t>
+  </si>
+  <si>
+    <t>0.010614, 35</t>
+  </si>
+  <si>
+    <t>0.12264, 68</t>
+  </si>
+  <si>
+    <t>5.866171908820763e-07, 50</t>
+  </si>
+  <si>
+    <t>0.0017, 34</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -798,6 +817,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -819,7 +845,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -828,7 +854,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -840,6 +865,14 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2479,8 +2512,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{46B8CD42-EC18-F248-9972-E237D48AFD0D}" name="Table10" displayName="Table10" ref="A61:D64" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
-  <autoFilter ref="A61:D64" xr:uid="{46B8CD42-EC18-F248-9972-E237D48AFD0D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{46B8CD42-EC18-F248-9972-E237D48AFD0D}" name="Table10" displayName="Table10" ref="A65:D68" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+  <autoFilter ref="A65:D68" xr:uid="{46B8CD42-EC18-F248-9972-E237D48AFD0D}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7165E551-4520-6046-BA0D-F388AB745054}" name="p value, ndrug" dataDxfId="40"/>
     <tableColumn id="2" xr3:uid="{3E6CE52F-8AC0-3447-B3E1-A7520AD09BBB}" name="NaCl (signed rank)" dataDxfId="39"/>
@@ -2492,8 +2525,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{CB6BB37A-DF8A-3F4A-8C7C-7068E706057F}" name="Table12" displayName="Table12" ref="A67:B70" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A67:B70" xr:uid="{CB6BB37A-DF8A-3F4A-8C7C-7068E706057F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{CB6BB37A-DF8A-3F4A-8C7C-7068E706057F}" name="Table12" displayName="Table12" ref="A71:B74" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A71:B74" xr:uid="{CB6BB37A-DF8A-3F4A-8C7C-7068E706057F}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C8666905-17ED-E042-AB5B-A635586A0533}" name="  " dataDxfId="34"/>
     <tableColumn id="2" xr3:uid="{758FE0DB-F9A7-1541-A892-83A3689CC2C6}" name="High vs Low FR (ranksum)" dataDxfId="33"/>
@@ -2503,8 +2536,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3AE76E7D-4BC1-9943-A996-E507FED1F25C}" name="Table13" displayName="Table13" ref="A73:D76" totalsRowShown="0" headerRowDxfId="32">
-  <autoFilter ref="A73:D76" xr:uid="{3AE76E7D-4BC1-9943-A996-E507FED1F25C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3AE76E7D-4BC1-9943-A996-E507FED1F25C}" name="Table13" displayName="Table13" ref="A77:D80" totalsRowShown="0" headerRowDxfId="32">
+  <autoFilter ref="A77:D80" xr:uid="{3AE76E7D-4BC1-9943-A996-E507FED1F25C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{2C045840-C761-AE4D-B9F3-D90E06487DD9}" name="p value, ndrug" dataDxfId="31"/>
     <tableColumn id="2" xr3:uid="{561FF46C-AC55-3B45-BF65-4D350423928A}" name="NaCl (signed rank)" dataDxfId="30"/>
@@ -2516,8 +2549,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E6DD0737-D28F-1F4C-B53C-A4A6EF25F271}" name="Table14" displayName="Table14" ref="A79:B82" totalsRowShown="0" headerRowDxfId="27">
-  <autoFilter ref="A79:B82" xr:uid="{E6DD0737-D28F-1F4C-B53C-A4A6EF25F271}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E6DD0737-D28F-1F4C-B53C-A4A6EF25F271}" name="Table14" displayName="Table14" ref="A83:B86" totalsRowShown="0" headerRowDxfId="27">
+  <autoFilter ref="A83:B86" xr:uid="{E6DD0737-D28F-1F4C-B53C-A4A6EF25F271}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{0C58147E-AC15-A545-BC38-F2E61BDA7CE8}" name=" " dataDxfId="26"/>
     <tableColumn id="2" xr3:uid="{8D6555BD-5093-5E4F-BFFF-C177158E876B}" name="High vs Low FR (ranksum)" dataDxfId="25"/>
@@ -2527,8 +2560,8 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{FF92885A-A117-BD46-9632-075EE49B7727}" name="Table15" displayName="Table15" ref="A86:D89" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A86:D89" xr:uid="{FF92885A-A117-BD46-9632-075EE49B7727}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{FF92885A-A117-BD46-9632-075EE49B7727}" name="Table15" displayName="Table15" ref="A90:D93" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A90:D93" xr:uid="{FF92885A-A117-BD46-9632-075EE49B7727}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{34D4DF3E-AE3E-464E-95DE-24DB9779A9AB}" name="p value, ndrug" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{BC707775-30D0-9342-B7C6-5C185C8EEE6E}" name="NaCl (signed rank)" dataDxfId="21"/>
@@ -2540,8 +2573,8 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{576E2118-EA50-7C4D-93BC-0242A2CED1BE}" name="Table16" displayName="Table16" ref="A92:D95" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A92:D95" xr:uid="{576E2118-EA50-7C4D-93BC-0242A2CED1BE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{576E2118-EA50-7C4D-93BC-0242A2CED1BE}" name="Table16" displayName="Table16" ref="A96:D99" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A96:D99" xr:uid="{576E2118-EA50-7C4D-93BC-0242A2CED1BE}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{CA2919BD-481D-D448-8C2E-8A5485FA04EF}" name="p value ndrug" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{F986C6D0-5537-9645-AD35-57B3AB94B930}" name="NaCl (signed rank)" dataDxfId="15"/>
@@ -2553,8 +2586,8 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{8D385D0E-135F-A14E-B1B1-9536609316A5}" name="Table17" displayName="Table17" ref="A98:H101" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A98:H101" xr:uid="{8D385D0E-135F-A14E-B1B1-9536609316A5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{8D385D0E-135F-A14E-B1B1-9536609316A5}" name="Table17" displayName="Table17" ref="A102:H105" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A102:H105" xr:uid="{8D385D0E-135F-A14E-B1B1-9536609316A5}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0CCDE9DC-9777-EB4A-8829-F2E258EB7A0F}" name="p value, ndrug" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{BD959637-C5F7-0445-8FF4-DC7235B73FD0}" name="NaCl (signed rank)" dataDxfId="9"/>
@@ -2570,8 +2603,8 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7EDA7C7F-35AD-BA40-B058-7A181082F834}" name="Table18" displayName="Table18" ref="A104:B107" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="A104:B107" xr:uid="{7EDA7C7F-35AD-BA40-B058-7A181082F834}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7EDA7C7F-35AD-BA40-B058-7A181082F834}" name="Table18" displayName="Table18" ref="A108:B111" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="A108:B111" xr:uid="{7EDA7C7F-35AD-BA40-B058-7A181082F834}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{696C77C0-F5D7-5C41-AD47-84D5D49BAD30}" name="  " dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{BB2D0153-FB2A-3B41-A087-4DC44031B8CE}" name="High vs Low FR (ranksum)" dataDxfId="0"/>
@@ -2632,8 +2665,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C5321602-2C62-6441-BD49-34843DC5EC9E}" name="Table6" displayName="Table6" ref="A36:D39" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
-  <autoFilter ref="A36:D39" xr:uid="{C5321602-2C62-6441-BD49-34843DC5EC9E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C5321602-2C62-6441-BD49-34843DC5EC9E}" name="Table6" displayName="Table6" ref="A40:D43" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
+  <autoFilter ref="A40:D43" xr:uid="{C5321602-2C62-6441-BD49-34843DC5EC9E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{1F814F2A-B411-9143-91B9-4B3599DB13CF}" name="p value, ndrug" dataDxfId="66"/>
     <tableColumn id="2" xr3:uid="{59D693D7-EB9E-2D41-AC3E-CA1A49B7DCE6}" name="NaCl (signed rank)" dataDxfId="65"/>
@@ -2645,8 +2678,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AF7CAE5F-4050-494B-8444-4010FD9A9503}" name="Table7" displayName="Table7" ref="A42:D45" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
-  <autoFilter ref="A42:D45" xr:uid="{AF7CAE5F-4050-494B-8444-4010FD9A9503}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AF7CAE5F-4050-494B-8444-4010FD9A9503}" name="Table7" displayName="Table7" ref="A46:D49" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+  <autoFilter ref="A46:D49" xr:uid="{AF7CAE5F-4050-494B-8444-4010FD9A9503}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8B916019-25D3-3D45-9925-267A0402C4F8}" name="p value, ndrug" dataDxfId="60"/>
     <tableColumn id="2" xr3:uid="{61736AC6-9797-5B48-B183-3B6215218DF8}" name="NaCl (signed rank)" dataDxfId="59"/>
@@ -2658,8 +2691,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0C5BDE58-1E6E-384C-A301-88BC3A7CF412}" name="Table8" displayName="Table8" ref="A48:H51" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
-  <autoFilter ref="A48:H51" xr:uid="{0C5BDE58-1E6E-384C-A301-88BC3A7CF412}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0C5BDE58-1E6E-384C-A301-88BC3A7CF412}" name="Table8" displayName="Table8" ref="A52:H55" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
+  <autoFilter ref="A52:H55" xr:uid="{0C5BDE58-1E6E-384C-A301-88BC3A7CF412}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{5EA9C801-7A12-FA47-9993-79019D358F40}" name="p value, ndrug" dataDxfId="54"/>
     <tableColumn id="2" xr3:uid="{B0AC27D2-E46F-DD43-A6E6-70FCFEC67CCF}" name="NaCl (signed rank)" dataDxfId="53"/>
@@ -2675,8 +2708,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{48CAD425-0C99-8048-AF71-3B8C84DE14B0}" name="Table9" displayName="Table9" ref="A54:B57" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
-  <autoFilter ref="A54:B57" xr:uid="{48CAD425-0C99-8048-AF71-3B8C84DE14B0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{48CAD425-0C99-8048-AF71-3B8C84DE14B0}" name="Table9" displayName="Table9" ref="A58:B61" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+  <autoFilter ref="A58:B61" xr:uid="{48CAD425-0C99-8048-AF71-3B8C84DE14B0}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{ABF2BE29-2111-6C46-AB1E-A3D7A182CFB9}" name="  " dataDxfId="44"/>
     <tableColumn id="2" xr3:uid="{C2EDD93A-A485-674E-B1D4-92AF4ADACF33}" name="High vs Low FR (ranksum)" dataDxfId="43"/>
@@ -2982,31 +3015,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7AD4EF-B60C-B945-BD48-3B2B2FC6C51E}">
-  <dimension ref="A3:H107"/>
+  <dimension ref="A3:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.5" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="4"/>
+    <col min="6" max="6" width="21.35546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="26.35546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.640625" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="10.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -3020,7 +3053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -3034,7 +3067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -3048,7 +3081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -3062,12 +3095,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -3078,45 +3111,45 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -3130,21 +3163,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -3152,32 +3185,32 @@
         <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>89</v>
+        <v>138</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -3191,57 +3224,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>74</v>
+        <v>124</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>91</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
         <v>25</v>
       </c>
@@ -3255,784 +3288,836 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D32" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E53" s="8">
+        <v>0.14030000000000001</v>
+      </c>
+      <c r="F53" s="8">
+        <v>0.64756000000000002</v>
+      </c>
+      <c r="G53" s="8">
+        <v>0.22037000000000001</v>
+      </c>
+      <c r="H53" s="8">
+        <v>0.41215000000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="8">
+        <v>0.84762000000000004</v>
+      </c>
+      <c r="F54" s="8">
+        <v>0.15237999999999999</v>
+      </c>
+      <c r="G54" s="8">
+        <v>0.72026999999999997</v>
+      </c>
+      <c r="H54" s="9">
+        <v>1.0702999999999999E-6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E55" s="8">
+        <v>0.24384</v>
+      </c>
+      <c r="F55" s="8">
+        <v>0.34561999999999998</v>
+      </c>
+      <c r="G55" s="8">
+        <v>0.54369000000000001</v>
+      </c>
+      <c r="H55" s="9">
+        <v>3.7367999999999999E-5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D78" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="79" spans="1:4">
+      <c r="A79" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D90" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+    <row r="91" spans="1:4">
+      <c r="A91" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="B91" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="B92" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
+      <c r="B93" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E102" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
+      <c r="F102" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
+      <c r="B103" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E103" s="3">
+        <v>0.28042</v>
+      </c>
+      <c r="F103" s="3">
+        <v>0.35341</v>
+      </c>
+      <c r="G103" s="3">
+        <v>3.5858999999999999E-3</v>
+      </c>
+      <c r="H103" s="3">
+        <v>0.98948000000000003</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
+      <c r="B104" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E104" s="3">
+        <v>0.60348000000000002</v>
+      </c>
+      <c r="F104" s="3">
+        <v>0.39651999999999998</v>
+      </c>
+      <c r="G104" s="3">
+        <v>0.72062000000000004</v>
+      </c>
+      <c r="H104" s="10">
+        <v>1.0519E-6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G48" s="7" t="s">
+      <c r="B105" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E105" s="3">
+        <v>0.30176999999999998</v>
+      </c>
+      <c r="F105" s="3">
+        <v>0.23913999999999999</v>
+      </c>
+      <c r="G105" s="3">
+        <v>0.46639999999999998</v>
+      </c>
+      <c r="H105" s="10">
+        <v>5.6138E-4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H48" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E49" s="9">
-        <v>0.16904</v>
-      </c>
-      <c r="F49" s="9">
-        <v>0.58089999999999997</v>
-      </c>
-      <c r="G49" s="9">
-        <v>0.20805999999999999</v>
-      </c>
-      <c r="H49" s="9">
-        <v>0.43936999999999998</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="9">
-        <v>0.87673999999999996</v>
-      </c>
-      <c r="F50" s="9">
-        <v>0.12325999999999999</v>
-      </c>
-      <c r="G50" s="9">
-        <v>0.71475999999999995</v>
-      </c>
-      <c r="H50" s="10">
-        <v>1.4107999999999999E-6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
+      <c r="B109" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B51" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="E51" s="9">
-        <v>0.25755</v>
-      </c>
-      <c r="F51" s="9">
-        <v>0.31829000000000002</v>
-      </c>
-      <c r="G51" s="9">
-        <v>0.53483999999999998</v>
-      </c>
-      <c r="H51" s="10">
-        <v>5.2726999999999998E-5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D74" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B87" s="3" t="s">
+      <c r="B111" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H98" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E99" s="3">
-        <v>0.28042</v>
-      </c>
-      <c r="F99" s="3">
-        <v>0.35341</v>
-      </c>
-      <c r="G99" s="3">
-        <v>3.5858999999999999E-3</v>
-      </c>
-      <c r="H99" s="3">
-        <v>0.98948000000000003</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E100" s="3">
-        <v>0.60348000000000002</v>
-      </c>
-      <c r="F100" s="3">
-        <v>0.39651999999999998</v>
-      </c>
-      <c r="G100" s="3">
-        <v>0.72062000000000004</v>
-      </c>
-      <c r="H100" s="11">
-        <v>1.0519E-6</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E101" s="3">
-        <v>0.30176999999999998</v>
-      </c>
-      <c r="F101" s="3">
-        <v>0.23913999999999999</v>
-      </c>
-      <c r="G101" s="3">
-        <v>0.46639999999999998</v>
-      </c>
-      <c r="H101" s="11">
-        <v>5.6138E-4</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="17">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -4049,6 +4134,7 @@
     <tablePart r:id="rId15"/>
     <tablePart r:id="rId16"/>
     <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Converted Fig. 4->5, Fig.S1->4
</commit_message>
<xml_diff>
--- a/resources/Data/p_value_tables.xlsx
+++ b/resources/Data/p_value_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\serotonin_project\to_github\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/My_Passport/serotonin_project/to_github/resources/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D77B7EB-DA9B-4EA5-A458-0719738B82AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA28AA4-92E9-AE4F-AD71-7EB5E9F76142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-111" yWindow="746" windowWidth="19748" windowHeight="13114" xr2:uid="{DF467324-0866-2946-B23A-F3365C304FA2}"/>
+    <workbookView xWindow="72000" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{DF467324-0866-2946-B23A-F3365C304FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -307,21 +307,6 @@
     </r>
   </si>
   <si>
-    <t>Figure 4 [MI Value: Drug Condition]</t>
-  </si>
-  <si>
-    <t>Figure 4 [Correlation: FR Control]</t>
-  </si>
-  <si>
-    <t>Figure 4 [Correlation: Drug Condition]</t>
-  </si>
-  <si>
-    <t>Figure 4 [MI Value: FR Control]</t>
-  </si>
-  <si>
-    <t>Figure S1B (E, F, G, H)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">1, 4 </t>
     </r>
@@ -338,9 +323,6 @@
   </si>
   <si>
     <t>0.83936, 13</t>
-  </si>
-  <si>
-    <t>Figure S1C</t>
   </si>
   <si>
     <r>
@@ -369,12 +351,6 @@
     <t>0.010195, 39</t>
   </si>
   <si>
-    <t>Figure S1D</t>
-  </si>
-  <si>
-    <t>Figure S1 (I &amp; J)</t>
-  </si>
-  <si>
     <t>Figure 2 (D &amp; H) (Gamma)</t>
   </si>
   <si>
@@ -734,12 +710,36 @@
   <si>
     <t>0.0017, 34</t>
   </si>
+  <si>
+    <t>Figure 4B (E, F, G, H)</t>
+  </si>
+  <si>
+    <t>Figure 4C</t>
+  </si>
+  <si>
+    <t>Figure 4D</t>
+  </si>
+  <si>
+    <t>Figure 4 (I &amp; J)</t>
+  </si>
+  <si>
+    <t>Figure 5 [Correlation: Drug Condition]</t>
+  </si>
+  <si>
+    <t>Figure 5 [Correlation: FR Control]</t>
+  </si>
+  <si>
+    <t>Figure 5 [MI Value: Drug Condition]</t>
+  </si>
+  <si>
+    <t>Figure 5 [MI Value: FR Control]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2512,8 +2512,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{46B8CD42-EC18-F248-9972-E237D48AFD0D}" name="Table10" displayName="Table10" ref="A65:D68" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
-  <autoFilter ref="A65:D68" xr:uid="{46B8CD42-EC18-F248-9972-E237D48AFD0D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{46B8CD42-EC18-F248-9972-E237D48AFD0D}" name="Table10" displayName="Table10" ref="A90:D93" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+  <autoFilter ref="A90:D93" xr:uid="{46B8CD42-EC18-F248-9972-E237D48AFD0D}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7165E551-4520-6046-BA0D-F388AB745054}" name="p value, ndrug" dataDxfId="40"/>
     <tableColumn id="2" xr3:uid="{3E6CE52F-8AC0-3447-B3E1-A7520AD09BBB}" name="NaCl (signed rank)" dataDxfId="39"/>
@@ -2525,8 +2525,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{CB6BB37A-DF8A-3F4A-8C7C-7068E706057F}" name="Table12" displayName="Table12" ref="A71:B74" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A71:B74" xr:uid="{CB6BB37A-DF8A-3F4A-8C7C-7068E706057F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{CB6BB37A-DF8A-3F4A-8C7C-7068E706057F}" name="Table12" displayName="Table12" ref="A96:B99" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A96:B99" xr:uid="{CB6BB37A-DF8A-3F4A-8C7C-7068E706057F}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C8666905-17ED-E042-AB5B-A635586A0533}" name="  " dataDxfId="34"/>
     <tableColumn id="2" xr3:uid="{758FE0DB-F9A7-1541-A892-83A3689CC2C6}" name="High vs Low FR (ranksum)" dataDxfId="33"/>
@@ -2536,8 +2536,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3AE76E7D-4BC1-9943-A996-E507FED1F25C}" name="Table13" displayName="Table13" ref="A77:D80" totalsRowShown="0" headerRowDxfId="32">
-  <autoFilter ref="A77:D80" xr:uid="{3AE76E7D-4BC1-9943-A996-E507FED1F25C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3AE76E7D-4BC1-9943-A996-E507FED1F25C}" name="Table13" displayName="Table13" ref="A102:D105" totalsRowShown="0" headerRowDxfId="32">
+  <autoFilter ref="A102:D105" xr:uid="{3AE76E7D-4BC1-9943-A996-E507FED1F25C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{2C045840-C761-AE4D-B9F3-D90E06487DD9}" name="p value, ndrug" dataDxfId="31"/>
     <tableColumn id="2" xr3:uid="{561FF46C-AC55-3B45-BF65-4D350423928A}" name="NaCl (signed rank)" dataDxfId="30"/>
@@ -2549,8 +2549,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E6DD0737-D28F-1F4C-B53C-A4A6EF25F271}" name="Table14" displayName="Table14" ref="A83:B86" totalsRowShown="0" headerRowDxfId="27">
-  <autoFilter ref="A83:B86" xr:uid="{E6DD0737-D28F-1F4C-B53C-A4A6EF25F271}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E6DD0737-D28F-1F4C-B53C-A4A6EF25F271}" name="Table14" displayName="Table14" ref="A108:B111" totalsRowShown="0" headerRowDxfId="27">
+  <autoFilter ref="A108:B111" xr:uid="{E6DD0737-D28F-1F4C-B53C-A4A6EF25F271}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{0C58147E-AC15-A545-BC38-F2E61BDA7CE8}" name=" " dataDxfId="26"/>
     <tableColumn id="2" xr3:uid="{8D6555BD-5093-5E4F-BFFF-C177158E876B}" name="High vs Low FR (ranksum)" dataDxfId="25"/>
@@ -2560,8 +2560,8 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{FF92885A-A117-BD46-9632-075EE49B7727}" name="Table15" displayName="Table15" ref="A90:D93" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A90:D93" xr:uid="{FF92885A-A117-BD46-9632-075EE49B7727}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{FF92885A-A117-BD46-9632-075EE49B7727}" name="Table15" displayName="Table15" ref="A65:D68" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A65:D68" xr:uid="{FF92885A-A117-BD46-9632-075EE49B7727}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{34D4DF3E-AE3E-464E-95DE-24DB9779A9AB}" name="p value, ndrug" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{BC707775-30D0-9342-B7C6-5C185C8EEE6E}" name="NaCl (signed rank)" dataDxfId="21"/>
@@ -2573,8 +2573,8 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{576E2118-EA50-7C4D-93BC-0242A2CED1BE}" name="Table16" displayName="Table16" ref="A96:D99" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A96:D99" xr:uid="{576E2118-EA50-7C4D-93BC-0242A2CED1BE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{576E2118-EA50-7C4D-93BC-0242A2CED1BE}" name="Table16" displayName="Table16" ref="A71:D74" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A71:D74" xr:uid="{576E2118-EA50-7C4D-93BC-0242A2CED1BE}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{CA2919BD-481D-D448-8C2E-8A5485FA04EF}" name="p value ndrug" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{F986C6D0-5537-9645-AD35-57B3AB94B930}" name="NaCl (signed rank)" dataDxfId="15"/>
@@ -2586,8 +2586,8 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{8D385D0E-135F-A14E-B1B1-9536609316A5}" name="Table17" displayName="Table17" ref="A102:H105" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A102:H105" xr:uid="{8D385D0E-135F-A14E-B1B1-9536609316A5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{8D385D0E-135F-A14E-B1B1-9536609316A5}" name="Table17" displayName="Table17" ref="A77:H80" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A77:H80" xr:uid="{8D385D0E-135F-A14E-B1B1-9536609316A5}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0CCDE9DC-9777-EB4A-8829-F2E258EB7A0F}" name="p value, ndrug" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{BD959637-C5F7-0445-8FF4-DC7235B73FD0}" name="NaCl (signed rank)" dataDxfId="9"/>
@@ -2603,8 +2603,8 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7EDA7C7F-35AD-BA40-B058-7A181082F834}" name="Table18" displayName="Table18" ref="A108:B111" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="A108:B111" xr:uid="{7EDA7C7F-35AD-BA40-B058-7A181082F834}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7EDA7C7F-35AD-BA40-B058-7A181082F834}" name="Table18" displayName="Table18" ref="A83:B86" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="A83:B86" xr:uid="{7EDA7C7F-35AD-BA40-B058-7A181082F834}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{696C77C0-F5D7-5C41-AD47-84D5D49BAD30}" name="  " dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{BB2D0153-FB2A-3B41-A087-4DC44031B8CE}" name="High vs Low FR (ranksum)" dataDxfId="0"/>
@@ -3017,29 +3017,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7AD4EF-B60C-B945-BD48-3B2B2FC6C51E}">
   <dimension ref="A3:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.5" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="21.35546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="26.35546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20.640625" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="10.85546875" style="4"/>
+    <col min="6" max="6" width="21.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -3095,12 +3095,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -3111,45 +3111,45 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -3174,10 +3174,10 @@
         <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -3185,32 +3185,32 @@
         <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -3224,57 +3224,57 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>25</v>
       </c>
@@ -3288,65 +3288,65 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="11" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>3</v>
       </c>
@@ -3354,40 +3354,40 @@
         <v>5</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>21</v>
       </c>
@@ -3401,21 +3401,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>7</v>
       </c>
@@ -3423,13 +3423,13 @@
         <v>30</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>11</v>
       </c>
@@ -3437,18 +3437,18 @@
         <v>29</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>36</v>
       </c>
@@ -3462,21 +3462,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>7</v>
       </c>
@@ -3484,32 +3484,32 @@
         <v>19</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>36</v>
       </c>
@@ -3535,18 +3535,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E53" s="8">
         <v>0.14030000000000001</v>
@@ -3561,7 +3561,7 @@
         <v>0.41215000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>7</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>40</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>10</v>
@@ -3587,18 +3587,18 @@
         <v>1.0702999999999999E-6</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="E55" s="8">
         <v>0.24384</v>
@@ -3613,12 +3613,12 @@
         <v>3.7367999999999999E-5</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>26</v>
       </c>
@@ -3626,36 +3626,36 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>21</v>
       </c>
@@ -3669,189 +3669,261 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
+        <v>0</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
+        <v>94</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
+        <v>19</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
+        <v>99</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B77" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C77" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D77" s="6" t="s">
+      <c r="D77" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="7" t="s">
+      <c r="E77" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B78" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="7" t="s">
+      <c r="B78" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E78" s="3">
+        <v>0.28042</v>
+      </c>
+      <c r="F78" s="3">
+        <v>0.35341</v>
+      </c>
+      <c r="G78" s="3">
+        <v>3.5858999999999999E-3</v>
+      </c>
+      <c r="H78" s="3">
+        <v>0.98948000000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B79" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="7" t="s">
+      <c r="B79" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E79" s="3">
+        <v>0.60348000000000002</v>
+      </c>
+      <c r="F79" s="3">
+        <v>0.39651999999999998</v>
+      </c>
+      <c r="G79" s="3">
+        <v>0.72062000000000004</v>
+      </c>
+      <c r="H79" s="10">
+        <v>1.0519E-6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B80" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="B80" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E80" s="3">
+        <v>0.30176999999999998</v>
+      </c>
+      <c r="F80" s="3">
+        <v>0.23913999999999999</v>
+      </c>
+      <c r="G80" s="3">
+        <v>0.46639999999999998</v>
+      </c>
+      <c r="H80" s="10">
+        <v>5.6138E-4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B83" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="7" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B86" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="B86" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>21</v>
       </c>
@@ -3865,253 +3937,181 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8">
-      <c r="A102" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B102" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B102" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D102" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E102" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G102" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H102" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8">
-      <c r="A103" s="2" t="s">
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B103" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E103" s="3">
-        <v>0.28042</v>
-      </c>
-      <c r="F103" s="3">
-        <v>0.35341</v>
-      </c>
-      <c r="G103" s="3">
-        <v>3.5858999999999999E-3</v>
-      </c>
-      <c r="H103" s="3">
-        <v>0.98948000000000003</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8">
-      <c r="A104" s="2" t="s">
+      <c r="B103" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B104" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E104" s="3">
-        <v>0.60348000000000002</v>
-      </c>
-      <c r="F104" s="3">
-        <v>0.39651999999999998</v>
-      </c>
-      <c r="G104" s="3">
-        <v>0.72062000000000004</v>
-      </c>
-      <c r="H104" s="10">
-        <v>1.0519E-6</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8">
-      <c r="A105" s="2" t="s">
+      <c r="B104" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B105" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E105" s="3">
-        <v>0.30176999999999998</v>
-      </c>
-      <c r="F105" s="3">
-        <v>0.23913999999999999</v>
-      </c>
-      <c r="G105" s="3">
-        <v>0.46639999999999998</v>
-      </c>
-      <c r="H105" s="10">
-        <v>5.6138E-4</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8">
+      <c r="B105" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8">
-      <c r="A108" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B108" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B108" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
-      <c r="A109" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8">
-      <c r="A110" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8">
-      <c r="A111" s="2" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B111" s="3" t="s">
-        <v>114</v>
+      <c r="B111" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>